<commit_message>
Hixe el primer cambio en el excel
</commit_message>
<xml_diff>
--- a/Inventario laboratorio de temperatura y humedad enero 2022.xlsx
+++ b/Inventario laboratorio de temperatura y humedad enero 2022.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\SENAMHI\Work\Dir 2022\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\GIT_Principal\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E0534F9C-E1C1-4D86-9CB3-A94E5BF4830A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F686E388-08EC-422F-9B71-5C3599888578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="705" yWindow="600" windowWidth="21600" windowHeight="11385" xr2:uid="{99E6FEA7-BD74-44FB-9B7A-77AC8AB8D313}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{99E6FEA7-BD74-44FB-9B7A-77AC8AB8D313}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="402" uniqueCount="230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="232">
   <si>
     <t>Inventario del laboratorio de termohigrometría</t>
   </si>
@@ -759,6 +759,12 @@
   </si>
   <si>
     <t>7ABTG046250</t>
+  </si>
+  <si>
+    <t>hola1</t>
+  </si>
+  <si>
+    <t>hola 2</t>
   </si>
 </sst>
 </file>
@@ -1188,7 +1194,7 @@
   <dimension ref="B1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="F98" sqref="F98"/>
+      <selection activeCell="B102" sqref="B102"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2863,9 +2869,15 @@
       <c r="F99" s="7"/>
     </row>
     <row r="100" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B100" s="2" t="s">
+        <v>230</v>
+      </c>
       <c r="F100" s="7"/>
     </row>
     <row r="101" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B101" s="2" t="s">
+        <v>231</v>
+      </c>
       <c r="F101" s="7"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Segundo cambio en txt y en el excel
</commit_message>
<xml_diff>
--- a/Inventario laboratorio de temperatura y humedad enero 2022.xlsx
+++ b/Inventario laboratorio de temperatura y humedad enero 2022.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\GIT_Principal\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F686E388-08EC-422F-9B71-5C3599888578}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F5D576-1E19-42F3-9D50-0D6555F4FE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{99E6FEA7-BD74-44FB-9B7A-77AC8AB8D313}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="234">
   <si>
     <t>Inventario del laboratorio de termohigrometría</t>
   </si>
@@ -765,6 +765,12 @@
   </si>
   <si>
     <t>hola 2</t>
+  </si>
+  <si>
+    <t>hola 11</t>
+  </si>
+  <si>
+    <t>hola 22</t>
   </si>
 </sst>
 </file>
@@ -1194,7 +1200,7 @@
   <dimension ref="B1:K103"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B102" sqref="B102"/>
+      <selection activeCell="B103" sqref="B103"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2881,9 +2887,15 @@
       <c r="F101" s="7"/>
     </row>
     <row r="102" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B102" s="2" t="s">
+        <v>232</v>
+      </c>
       <c r="F102" s="7"/>
     </row>
     <row r="103" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B103" s="2" t="s">
+        <v>233</v>
+      </c>
       <c r="F103" s="7"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cambios en los 4 documentos
</commit_message>
<xml_diff>
--- a/Inventario laboratorio de temperatura y humedad enero 2022.xlsx
+++ b/Inventario laboratorio de temperatura y humedad enero 2022.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Desktop\GIT_Principal\P1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0F5D576-1E19-42F3-9D50-0D6555F4FE2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82C1EBF5-C86F-45CC-82F3-85C7E8B07426}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{99E6FEA7-BD74-44FB-9B7A-77AC8AB8D313}"/>
+    <workbookView xWindow="31200" yWindow="1800" windowWidth="21600" windowHeight="11385" xr2:uid="{99E6FEA7-BD74-44FB-9B7A-77AC8AB8D313}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="406" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="237">
   <si>
     <t>Inventario del laboratorio de termohigrometría</t>
   </si>
@@ -771,6 +771,15 @@
   </si>
   <si>
     <t>hola 22</t>
+  </si>
+  <si>
+    <t>hola 33</t>
+  </si>
+  <si>
+    <t>hola 34</t>
+  </si>
+  <si>
+    <t>hola 35</t>
   </si>
 </sst>
 </file>
@@ -1197,10 +1206,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52EA4913-57E9-4200-BBFB-97C706D3BBD6}">
-  <dimension ref="B1:K103"/>
+  <dimension ref="B1:K106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection activeCell="B103" sqref="B103"/>
+    <sheetView tabSelected="1" topLeftCell="A92" workbookViewId="0">
+      <selection activeCell="B107" sqref="B107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2898,6 +2907,21 @@
       </c>
       <c r="F103" s="7"/>
     </row>
+    <row r="104" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B104" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="105" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B105" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="106" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B106" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>